<commit_message>
fix choose_next on brute_force. no need to remove after choose random
</commit_message>
<xml_diff>
--- a/Semantle_AI/New_service/Reports_output/Priority_calculation/error_calc_compare.xlsx
+++ b/Semantle_AI/New_service/Reports_output/Priority_calculation/error_calc_compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bardamri/PycharmProjects/SE_Project_Semantle/Semantle_AI/New_service/Reports_output/Priority_calculation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2667CCA7-757D-3247-A9FE-7BAF5A944F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62710271-6183-8D4A-8390-ACF2DCD2CF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{2BD9F7E4-3864-E14D-AD8C-55EBE9E46C48}"/>
   </bookViews>
@@ -182,12 +182,6 @@
     <t>words</t>
   </si>
   <si>
-    <t>Sum relative * Sum vector</t>
-  </si>
-  <si>
-    <t>SUM * Sum vec</t>
-  </si>
-  <si>
     <t>Brute force</t>
   </si>
   <si>
@@ -198,6 +192,12 @@
   </si>
   <si>
     <t>Prob</t>
+  </si>
+  <si>
+    <t>Sum relative * Norm1</t>
+  </si>
+  <si>
+    <t>SUM * Norm1</t>
   </si>
 </sst>
 </file>
@@ -434,10 +434,10 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>SUM * Sum vec</c:v>
+                  <c:v>SUM * Norm1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Sum relative * Sum vector</c:v>
+                  <c:v>Sum relative * Norm1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Brute force</c:v>
@@ -866,10 +866,10 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>SUM * Sum vec</c:v>
+                  <c:v>SUM * Norm1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Sum relative * Sum vector</c:v>
+                  <c:v>Sum relative * Norm1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Brute force</c:v>
@@ -1230,10 +1230,10 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>SUM * Sum vec</c:v>
+                  <c:v>SUM * Norm1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Sum relative * Sum vector</c:v>
+                  <c:v>Sum relative * Norm1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Brute force</c:v>
@@ -1602,10 +1602,10 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>SUM * Sum vec</c:v>
+                  <c:v>SUM * Norm1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Sum relative * Sum vector</c:v>
+                  <c:v>Sum relative * Norm1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Brute force</c:v>
@@ -4600,16 +4600,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08AAC9F3-9758-EE4C-9725-9BEBC9FEF52E}">
   <dimension ref="A1:N1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="8" max="8" width="33.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -4622,22 +4622,22 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>47</v>
@@ -4832,7 +4832,7 @@
       </c>
       <c r="H8" t="str">
         <f>A1</f>
-        <v>SUM * Sum vec</v>
+        <v>SUM * Norm1</v>
       </c>
       <c r="I8" s="4">
         <f>AVERAGE(A2:A501)</f>
@@ -4883,7 +4883,7 @@
       </c>
       <c r="H9" t="str">
         <f>B1</f>
-        <v>Sum relative * Sum vector</v>
+        <v>Sum relative * Norm1</v>
       </c>
       <c r="I9" s="4">
         <f>AVERAGE(B2:B501)</f>

</xml_diff>

<commit_message>
editing voi for k numbers. select k random probabilities. fix random for range.
</commit_message>
<xml_diff>
--- a/Semantle_AI/New_service/Reports_output/Priority_calculation/error_calc_compare.xlsx
+++ b/Semantle_AI/New_service/Reports_output/Priority_calculation/error_calc_compare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bardamri/PycharmProjects/SE_Project_Semantle/Semantle_AI/New_service/Reports_output/Priority_calculation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62710271-6183-8D4A-8390-ACF2DCD2CF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA7709B-3F49-B748-9AA0-2F79A871F18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{2BD9F7E4-3864-E14D-AD8C-55EBE9E46C48}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{2BD9F7E4-3864-E14D-AD8C-55EBE9E46C48}"/>
   </bookViews>
   <sheets>
     <sheet name="GLOVE_FASTTEXT" sheetId="2" r:id="rId1"/>
@@ -59,126 +59,6 @@
     <t>MAX VALUE</t>
   </si>
   <si>
-    <t>columnist</t>
-  </si>
-  <si>
-    <t>university</t>
-  </si>
-  <si>
-    <t>readily</t>
-  </si>
-  <si>
-    <t>painting</t>
-  </si>
-  <si>
-    <t>tourist</t>
-  </si>
-  <si>
-    <t>advocate</t>
-  </si>
-  <si>
-    <t>send</t>
-  </si>
-  <si>
-    <t>neighboring</t>
-  </si>
-  <si>
-    <t>oven</t>
-  </si>
-  <si>
-    <t>know</t>
-  </si>
-  <si>
-    <t>opposition</t>
-  </si>
-  <si>
-    <t>trait</t>
-  </si>
-  <si>
-    <t>worker</t>
-  </si>
-  <si>
-    <t>honey</t>
-  </si>
-  <si>
-    <t>candidate</t>
-  </si>
-  <si>
-    <t>initiate</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>opponent</t>
-  </si>
-  <si>
-    <t>deny</t>
-  </si>
-  <si>
-    <t>secret</t>
-  </si>
-  <si>
-    <t>ownership</t>
-  </si>
-  <si>
-    <t>morning</t>
-  </si>
-  <si>
-    <t>southern</t>
-  </si>
-  <si>
-    <t>suppose</t>
-  </si>
-  <si>
-    <t>oppose</t>
-  </si>
-  <si>
-    <t>gut</t>
-  </si>
-  <si>
-    <t>bottom</t>
-  </si>
-  <si>
-    <t>rhythm</t>
-  </si>
-  <si>
-    <t>particle</t>
-  </si>
-  <si>
-    <t>cancel</t>
-  </si>
-  <si>
-    <t>bee</t>
-  </si>
-  <si>
-    <t>separate</t>
-  </si>
-  <si>
-    <t>war</t>
-  </si>
-  <si>
-    <t>staff</t>
-  </si>
-  <si>
-    <t>notion</t>
-  </si>
-  <si>
-    <t>till</t>
-  </si>
-  <si>
-    <t>drug</t>
-  </si>
-  <si>
-    <t>travel</t>
-  </si>
-  <si>
-    <t>prefer</t>
-  </si>
-  <si>
-    <t>invention</t>
-  </si>
-  <si>
     <t>words</t>
   </si>
   <si>
@@ -198,6 +78,126 @@
   </si>
   <si>
     <t>SUM * Norm1</t>
+  </si>
+  <si>
+    <t>ultimately</t>
+  </si>
+  <si>
+    <t>encouraging</t>
+  </si>
+  <si>
+    <t>merely</t>
+  </si>
+  <si>
+    <t>lemon</t>
+  </si>
+  <si>
+    <t>derive</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>bed</t>
+  </si>
+  <si>
+    <t>sculpture</t>
+  </si>
+  <si>
+    <t>primarily</t>
+  </si>
+  <si>
+    <t>tolerate</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>mechanism</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>odd</t>
+  </si>
+  <si>
+    <t>developer</t>
+  </si>
+  <si>
+    <t>poster</t>
+  </si>
+  <si>
+    <t>situation</t>
+  </si>
+  <si>
+    <t>ironically</t>
+  </si>
+  <si>
+    <t>king</t>
+  </si>
+  <si>
+    <t>influence</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>seminar</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>school</t>
+  </si>
+  <si>
+    <t>terrible</t>
+  </si>
+  <si>
+    <t>produce</t>
+  </si>
+  <si>
+    <t>remaining</t>
+  </si>
+  <si>
+    <t>guilt</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>tail</t>
+  </si>
+  <si>
+    <t>fragile</t>
+  </si>
+  <si>
+    <t>ceiling</t>
+  </si>
+  <si>
+    <t>golf</t>
+  </si>
+  <si>
+    <t>contemporary</t>
+  </si>
+  <si>
+    <t>visible</t>
+  </si>
+  <si>
+    <t>absolute</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>painter</t>
+  </si>
+  <si>
+    <t>threaten</t>
   </si>
 </sst>
 </file>
@@ -461,16 +461,16 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2040.425</c:v>
+                  <c:v>2454.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2275.9250000000002</c:v>
+                  <c:v>2473.9250000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1985.2</c:v>
+                  <c:v>2229.4749999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2451.6999999999998</c:v>
+                  <c:v>2471.65</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1831.4</c:v>
@@ -893,16 +893,16 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1984.5</c:v>
+                  <c:v>2846</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2334</c:v>
+                  <c:v>2799</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2262.5</c:v>
+                  <c:v>2420</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2860.5</c:v>
+                  <c:v>2851.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1831.4</c:v>
@@ -1257,19 +1257,19 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1311944.2506410258</c:v>
+                  <c:v>1561295.1692307692</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1231645.4655870441</c:v>
+                  <c:v>1532905.5182186232</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1264439.1073968709</c:v>
+                  <c:v>1515245.8890469421</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1294361.4789789792</c:v>
+                  <c:v>1551115.696696697</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1317382.2285714287</c:v>
+                  <c:v>1514862.3111111112</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1046064.8455128204</c:v>
@@ -1629,16 +1629,16 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1145.4010000000001</c:v>
+                  <c:v>1249.518</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1150.9670000000001</c:v>
+                  <c:v>1242.3330000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1230.8399999999999</c:v>
+                  <c:v>1256.9459999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1238.825</c:v>
+                  <c:v>1246.8699999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1378.3409999999999</c:v>
@@ -4601,16 +4601,18 @@
   <dimension ref="A1:N1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
@@ -4622,39 +4624,39 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>4103</v>
+        <v>4059</v>
       </c>
       <c r="B2" s="1">
-        <v>4145</v>
+        <v>4044</v>
       </c>
       <c r="C2" s="1">
-        <v>1949</v>
+        <v>366</v>
       </c>
       <c r="D2" s="1">
-        <v>4053</v>
+        <v>4052</v>
       </c>
       <c r="E2" s="1">
         <v>4119</v>
@@ -4663,21 +4665,21 @@
         <v>62</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>2121</v>
+        <v>3873</v>
       </c>
       <c r="B3" s="1">
-        <v>2494</v>
+        <v>3805</v>
       </c>
       <c r="C3" s="1">
-        <v>3010</v>
+        <v>121</v>
       </c>
       <c r="D3" s="1">
-        <v>3895</v>
+        <v>3844</v>
       </c>
       <c r="E3" s="1">
         <v>2049</v>
@@ -4686,18 +4688,18 @@
         <v>244</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>2411</v>
+        <v>2842</v>
       </c>
       <c r="B4" s="1">
-        <v>2956</v>
+        <v>2806</v>
       </c>
       <c r="C4" s="1">
-        <v>201</v>
+        <v>3001</v>
       </c>
       <c r="D4" s="1">
         <v>2820</v>
@@ -4709,20 +4711,20 @@
         <v>1028</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>2662</v>
+        <v>706</v>
       </c>
       <c r="B5" s="1">
-        <v>2880</v>
+        <v>565</v>
       </c>
       <c r="C5" s="1">
-        <v>1651</v>
+        <v>863</v>
       </c>
       <c r="D5" s="1">
         <v>619</v>
@@ -4734,23 +4736,23 @@
         <v>2474</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>2459</v>
+        <v>1997</v>
       </c>
       <c r="B6" s="1">
-        <v>2756</v>
+        <v>1990</v>
       </c>
       <c r="C6" s="1">
-        <v>2576</v>
+        <v>2526</v>
       </c>
       <c r="D6" s="1">
-        <v>1949</v>
+        <v>2003</v>
       </c>
       <c r="E6" s="1">
         <v>2393</v>
@@ -4759,23 +4761,23 @@
         <v>1109</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>2198</v>
+        <v>3096</v>
       </c>
       <c r="B7" s="1">
-        <v>2724</v>
+        <v>3076</v>
       </c>
       <c r="C7" s="1">
-        <v>3678</v>
+        <v>2670</v>
       </c>
       <c r="D7" s="1">
-        <v>3043</v>
+        <v>3157</v>
       </c>
       <c r="E7" s="1">
         <v>2327</v>
@@ -4784,7 +4786,7 @@
         <v>2180</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
         <v>0</v>
@@ -4810,16 +4812,16 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>711</v>
+        <v>211</v>
       </c>
       <c r="B8" s="1">
-        <v>1016</v>
+        <v>241</v>
       </c>
       <c r="C8" s="1">
-        <v>1777</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1">
-        <v>292</v>
+        <v>255</v>
       </c>
       <c r="E8" s="1">
         <v>87</v>
@@ -4828,7 +4830,7 @@
         <v>2931</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H8" t="str">
         <f>A1</f>
@@ -4836,41 +4838,41 @@
       </c>
       <c r="I8" s="4">
         <f>AVERAGE(A2:A501)</f>
-        <v>2040.425</v>
+        <v>2454.6</v>
       </c>
       <c r="J8" s="4">
         <f>MEDIAN(A1:A501)</f>
-        <v>1984.5</v>
+        <v>2846</v>
       </c>
       <c r="K8" s="4">
         <f>VAR(A2:A501)</f>
-        <v>1311944.2506410258</v>
+        <v>1561295.1692307692</v>
       </c>
       <c r="L8" s="4">
         <f>ROUND(STDEV(A2:A501),3)</f>
-        <v>1145.4010000000001</v>
+        <v>1249.518</v>
       </c>
       <c r="M8">
         <f>MIN(A2:A501)</f>
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N8">
         <f>MAX(A2:A501)</f>
-        <v>4106</v>
+        <v>4138</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>2160</v>
+        <v>2932</v>
       </c>
       <c r="B9" s="1">
-        <v>2574</v>
+        <v>2903</v>
       </c>
       <c r="C9" s="1">
-        <v>2828</v>
+        <v>4124</v>
       </c>
       <c r="D9" s="1">
-        <v>2967</v>
+        <v>2938</v>
       </c>
       <c r="E9" s="1">
         <v>2140</v>
@@ -4879,7 +4881,7 @@
         <v>2895</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H9" t="str">
         <f>B1</f>
@@ -4887,41 +4889,41 @@
       </c>
       <c r="I9" s="4">
         <f>AVERAGE(B2:B501)</f>
-        <v>2275.9250000000002</v>
+        <v>2473.9250000000002</v>
       </c>
       <c r="J9" s="4">
         <f>MEDIAN(B2:B501)</f>
-        <v>2334</v>
+        <v>2799</v>
       </c>
       <c r="K9" s="4">
         <f>VAR(A3:A502)</f>
-        <v>1231645.4655870441</v>
+        <v>1532905.5182186232</v>
       </c>
       <c r="L9" s="4">
         <f>ROUND(STDEV(B2:B501),3)</f>
-        <v>1150.9670000000001</v>
+        <v>1242.3330000000001</v>
       </c>
       <c r="M9">
         <f>MIN(B2:B501)</f>
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="N9">
         <f>MAX(B2:B501)</f>
-        <v>4145</v>
+        <v>4143</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>3946</v>
+        <v>3934</v>
       </c>
       <c r="B10" s="1">
-        <v>4023</v>
+        <v>3880</v>
       </c>
       <c r="C10" s="1">
-        <v>3350</v>
+        <v>1313</v>
       </c>
       <c r="D10" s="1">
-        <v>3771</v>
+        <v>3916</v>
       </c>
       <c r="E10" s="1">
         <v>3955</v>
@@ -4930,7 +4932,7 @@
         <v>189</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H10" t="str">
         <f>C1</f>
@@ -4938,41 +4940,41 @@
       </c>
       <c r="I10" s="4">
         <f>AVERAGE(C2:C501)</f>
-        <v>1985.2</v>
+        <v>2229.4749999999999</v>
       </c>
       <c r="J10" s="4">
         <f>MEDIAN(C2:C501)</f>
-        <v>2262.5</v>
+        <v>2420</v>
       </c>
       <c r="K10" s="4">
         <f>VAR(A4:A503)</f>
-        <v>1264439.1073968709</v>
+        <v>1515245.8890469421</v>
       </c>
       <c r="L10" s="4">
         <f>ROUND(STDEV(C2:C501),3)</f>
-        <v>1230.8399999999999</v>
+        <v>1256.9459999999999</v>
       </c>
       <c r="M10">
         <f>MIN(C2:C501)</f>
-        <v>125</v>
+        <v>45</v>
       </c>
       <c r="N10">
         <f>MAX(C2:C501)</f>
-        <v>3860</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>88</v>
+        <v>2358</v>
       </c>
       <c r="B11" s="1">
-        <v>68</v>
+        <v>2415</v>
       </c>
       <c r="C11" s="1">
-        <v>362</v>
+        <v>2430</v>
       </c>
       <c r="D11" s="1">
-        <v>2198</v>
+        <v>2468</v>
       </c>
       <c r="E11" s="1">
         <v>117</v>
@@ -4981,7 +4983,7 @@
         <v>1227</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="H11" t="str">
         <f>D1</f>
@@ -4989,19 +4991,19 @@
       </c>
       <c r="I11" s="4">
         <f>AVERAGE(D2:D501)</f>
-        <v>2451.6999999999998</v>
+        <v>2471.65</v>
       </c>
       <c r="J11" s="4">
         <f>MEDIAN(D2:D501)</f>
-        <v>2860.5</v>
+        <v>2851.5</v>
       </c>
       <c r="K11" s="4">
         <f>VAR(A5:A504)</f>
-        <v>1294361.4789789792</v>
+        <v>1551115.696696697</v>
       </c>
       <c r="L11" s="4">
         <f>ROUND(STDEV(D2:D501),3)</f>
-        <v>1238.825</v>
+        <v>1246.8699999999999</v>
       </c>
       <c r="M11">
         <f>MIN(D2:D501)</f>
@@ -5009,21 +5011,21 @@
       </c>
       <c r="N11">
         <f>MAX(D2:D501)</f>
-        <v>4135</v>
+        <v>4133</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>912</v>
+        <v>1091</v>
       </c>
       <c r="B12" s="1">
-        <v>1389</v>
+        <v>1268</v>
       </c>
       <c r="C12" s="1">
-        <v>1787</v>
+        <v>1196</v>
       </c>
       <c r="D12" s="1">
-        <v>1231</v>
+        <v>1141</v>
       </c>
       <c r="E12" s="1">
         <v>744</v>
@@ -5032,7 +5034,7 @@
         <v>1587</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H12" t="str">
         <f>E1</f>
@@ -5048,7 +5050,7 @@
       </c>
       <c r="K12" s="4">
         <f>VAR(A6:A505)</f>
-        <v>1317382.2285714287</v>
+        <v>1514862.3111111112</v>
       </c>
       <c r="L12" s="4">
         <f>ROUND(STDEV(E2:E501),3)</f>
@@ -5065,16 +5067,16 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>3801</v>
+        <v>3467</v>
       </c>
       <c r="B13" s="1">
-        <v>4014</v>
+        <v>3547</v>
       </c>
       <c r="C13" s="1">
-        <v>3105</v>
+        <v>2191</v>
       </c>
       <c r="D13" s="1">
-        <v>3542</v>
+        <v>3540</v>
       </c>
       <c r="E13" s="1">
         <v>3959</v>
@@ -5083,7 +5085,7 @@
         <v>837</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H13" t="str">
         <f>F1</f>
@@ -5116,16 +5118,16 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>1988</v>
+        <v>3063</v>
       </c>
       <c r="B14" s="1">
-        <v>2311</v>
+        <v>3081</v>
       </c>
       <c r="C14" s="1">
-        <v>2778</v>
+        <v>1229</v>
       </c>
       <c r="D14" s="1">
-        <v>2997</v>
+        <v>2989</v>
       </c>
       <c r="E14" s="1">
         <v>1633</v>
@@ -5134,18 +5136,18 @@
         <v>1725</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>3923</v>
+        <v>86</v>
       </c>
       <c r="B15" s="1">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="C15" s="1">
-        <v>3860</v>
+        <v>2365</v>
       </c>
       <c r="D15" s="1">
         <v>92</v>
@@ -5157,21 +5159,21 @@
         <v>2918</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>1571</v>
+        <v>3121</v>
       </c>
       <c r="B16" s="1">
-        <v>2062</v>
+        <v>2997</v>
       </c>
       <c r="C16" s="1">
-        <v>2963</v>
+        <v>450</v>
       </c>
       <c r="D16" s="1">
-        <v>3128</v>
+        <v>3171</v>
       </c>
       <c r="E16" s="1">
         <v>1443</v>
@@ -5180,21 +5182,21 @@
         <v>608</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>2189</v>
+        <v>1687</v>
       </c>
       <c r="B17" s="1">
-        <v>3277</v>
+        <v>1763</v>
       </c>
       <c r="C17" s="1">
-        <v>1419</v>
+        <v>1759</v>
       </c>
       <c r="D17" s="1">
-        <v>1751</v>
+        <v>1791</v>
       </c>
       <c r="E17" s="1">
         <v>2860</v>
@@ -5203,21 +5205,21 @@
         <v>2916</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>664</v>
+        <v>3945</v>
       </c>
       <c r="B18" s="1">
-        <v>928</v>
+        <v>3997</v>
       </c>
       <c r="C18" s="1">
-        <v>3599</v>
+        <v>2410</v>
       </c>
       <c r="D18" s="1">
-        <v>3939</v>
+        <v>3998</v>
       </c>
       <c r="E18" s="1">
         <v>202</v>
@@ -5226,21 +5228,21 @@
         <v>226</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>1981</v>
+        <v>4041</v>
       </c>
       <c r="B19" s="1">
-        <v>2411</v>
+        <v>4048</v>
       </c>
       <c r="C19" s="1">
-        <v>125</v>
+        <v>3768</v>
       </c>
       <c r="D19" s="1">
-        <v>3989</v>
+        <v>4030</v>
       </c>
       <c r="E19" s="1">
         <v>1964</v>
@@ -5249,18 +5251,18 @@
         <v>243</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>1451</v>
+        <v>964</v>
       </c>
       <c r="B20" s="1">
-        <v>2357</v>
+        <v>1029</v>
       </c>
       <c r="C20" s="1">
-        <v>1616</v>
+        <v>951</v>
       </c>
       <c r="D20" s="1">
         <v>1019</v>
@@ -5272,21 +5274,21 @@
         <v>2888</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>1299</v>
+        <v>3664</v>
       </c>
       <c r="B21" s="1">
-        <v>1524</v>
+        <v>3835</v>
       </c>
       <c r="C21" s="1">
-        <v>2958</v>
+        <v>1717</v>
       </c>
       <c r="D21" s="1">
-        <v>3703</v>
+        <v>3653</v>
       </c>
       <c r="E21" s="1">
         <v>1150</v>
@@ -5295,21 +5297,21 @@
         <v>480</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>1301</v>
+        <v>2714</v>
       </c>
       <c r="B22" s="1">
-        <v>1689</v>
+        <v>2594</v>
       </c>
       <c r="C22" s="1">
-        <v>305</v>
+        <v>3945</v>
       </c>
       <c r="D22" s="1">
-        <v>2587</v>
+        <v>2704</v>
       </c>
       <c r="E22" s="1">
         <v>659</v>
@@ -5318,18 +5320,18 @@
         <v>1076</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>1380</v>
+        <v>273</v>
       </c>
       <c r="B23" s="1">
-        <v>1818</v>
+        <v>355</v>
       </c>
       <c r="C23" s="1">
-        <v>2654</v>
+        <v>3077</v>
       </c>
       <c r="D23" s="1">
         <v>277</v>
@@ -5341,21 +5343,21 @@
         <v>2925</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>1800</v>
+        <v>2258</v>
       </c>
       <c r="B24" s="1">
-        <v>2131</v>
+        <v>2319</v>
       </c>
       <c r="C24" s="1">
-        <v>3167</v>
+        <v>3748</v>
       </c>
       <c r="D24" s="1">
-        <v>2269</v>
+        <v>2359</v>
       </c>
       <c r="E24" s="1">
         <v>972</v>
@@ -5364,21 +5366,21 @@
         <v>1332</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>2511</v>
+        <v>3084</v>
       </c>
       <c r="B25" s="1">
-        <v>3141</v>
+        <v>3005</v>
       </c>
       <c r="C25" s="1">
-        <v>276</v>
+        <v>3306</v>
       </c>
       <c r="D25" s="1">
-        <v>2979</v>
+        <v>3113</v>
       </c>
       <c r="E25" s="1">
         <v>2994</v>
@@ -5387,21 +5389,21 @@
         <v>685</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>1171</v>
+        <v>2431</v>
       </c>
       <c r="B26" s="1">
-        <v>1765</v>
+        <v>2576</v>
       </c>
       <c r="C26" s="1">
-        <v>129</v>
+        <v>2619</v>
       </c>
       <c r="D26" s="1">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="E26" s="1">
         <v>1195</v>
@@ -5410,21 +5412,21 @@
         <v>2504</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>3708</v>
+        <v>3360</v>
       </c>
       <c r="B27" s="1">
-        <v>3852</v>
+        <v>3545</v>
       </c>
       <c r="C27" s="1">
-        <v>3681</v>
+        <v>4142</v>
       </c>
       <c r="D27" s="1">
-        <v>3399</v>
+        <v>3368</v>
       </c>
       <c r="E27" s="1">
         <v>3722</v>
@@ -5433,18 +5435,18 @@
         <v>514</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>1817</v>
+        <v>2949</v>
       </c>
       <c r="B28" s="1">
-        <v>2016</v>
+        <v>2954</v>
       </c>
       <c r="C28" s="1">
-        <v>532</v>
+        <v>3011</v>
       </c>
       <c r="D28" s="1">
         <v>2927</v>
@@ -5456,21 +5458,21 @@
         <v>1389</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>3254</v>
+        <v>3753</v>
       </c>
       <c r="B29" s="1">
-        <v>3519</v>
+        <v>3794</v>
       </c>
       <c r="C29" s="1">
-        <v>156</v>
+        <v>222</v>
       </c>
       <c r="D29" s="1">
-        <v>3751</v>
+        <v>3759</v>
       </c>
       <c r="E29" s="1">
         <v>3345</v>
@@ -5479,21 +5481,21 @@
         <v>550</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>3812</v>
+        <v>659</v>
       </c>
       <c r="B30" s="1">
-        <v>3937</v>
+        <v>658</v>
       </c>
       <c r="C30" s="1">
-        <v>1275</v>
+        <v>1800</v>
       </c>
       <c r="D30" s="1">
-        <v>685</v>
+        <v>678</v>
       </c>
       <c r="E30" s="1">
         <v>3859</v>
@@ -5502,21 +5504,21 @@
         <v>2638</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>2626</v>
+        <v>3793</v>
       </c>
       <c r="B31" s="1">
-        <v>3258</v>
+        <v>3835</v>
       </c>
       <c r="C31" s="1">
-        <v>776</v>
+        <v>2785</v>
       </c>
       <c r="D31" s="1">
-        <v>3781</v>
+        <v>3798</v>
       </c>
       <c r="E31" s="1">
         <v>2782</v>
@@ -5525,21 +5527,21 @@
         <v>538</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>4106</v>
+        <v>734</v>
       </c>
       <c r="B32" s="1">
-        <v>4121</v>
+        <v>818</v>
       </c>
       <c r="C32" s="1">
-        <v>225</v>
+        <v>1569</v>
       </c>
       <c r="D32" s="1">
-        <v>664</v>
+        <v>687</v>
       </c>
       <c r="E32" s="1">
         <v>4074</v>
@@ -5548,18 +5550,18 @@
         <v>2933</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>633</v>
+        <v>1874</v>
       </c>
       <c r="B33" s="1">
-        <v>696</v>
+        <v>2034</v>
       </c>
       <c r="C33" s="1">
-        <v>2598</v>
+        <v>3683</v>
       </c>
       <c r="D33" s="1">
         <v>2070</v>
@@ -5571,18 +5573,18 @@
         <v>2938</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>649</v>
+        <v>1765</v>
       </c>
       <c r="B34" s="1">
-        <v>743</v>
+        <v>1788</v>
       </c>
       <c r="C34" s="1">
-        <v>3134</v>
+        <v>3869</v>
       </c>
       <c r="D34" s="1">
         <v>1721</v>
@@ -5594,21 +5596,21 @@
         <v>1574</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>1265</v>
+        <v>142</v>
       </c>
       <c r="B35" s="1">
-        <v>1473</v>
+        <v>92</v>
       </c>
       <c r="C35" s="1">
-        <v>3116</v>
+        <v>3043</v>
       </c>
       <c r="D35" s="1">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="E35" s="1">
         <v>741</v>
@@ -5617,21 +5619,21 @@
         <v>2282</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>654</v>
+        <v>4138</v>
       </c>
       <c r="B36" s="1">
-        <v>1063</v>
+        <v>4143</v>
       </c>
       <c r="C36" s="1">
-        <v>1662</v>
+        <v>1138</v>
       </c>
       <c r="D36" s="1">
-        <v>4135</v>
+        <v>4133</v>
       </c>
       <c r="E36" s="1">
         <v>330</v>
@@ -5640,21 +5642,21 @@
         <v>64</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>2673</v>
+        <v>2850</v>
       </c>
       <c r="B37" s="1">
-        <v>3028</v>
+        <v>2792</v>
       </c>
       <c r="C37" s="1">
-        <v>770</v>
+        <v>2785</v>
       </c>
       <c r="D37" s="1">
-        <v>2901</v>
+        <v>2900</v>
       </c>
       <c r="E37" s="1">
         <v>2466</v>
@@ -5663,21 +5665,21 @@
         <v>744</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>1263</v>
+        <v>3405</v>
       </c>
       <c r="B38" s="1">
-        <v>1415</v>
+        <v>3403</v>
       </c>
       <c r="C38" s="1">
-        <v>2774</v>
+        <v>1558</v>
       </c>
       <c r="D38" s="1">
-        <v>3370</v>
+        <v>3367</v>
       </c>
       <c r="E38" s="1">
         <v>854</v>
@@ -5686,21 +5688,21 @@
         <v>2947</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>830</v>
+        <v>1849</v>
       </c>
       <c r="B39" s="1">
-        <v>961</v>
+        <v>1883</v>
       </c>
       <c r="C39" s="1">
-        <v>2667</v>
+        <v>3829</v>
       </c>
       <c r="D39" s="1">
-        <v>1892</v>
+        <v>1867</v>
       </c>
       <c r="E39" s="1">
         <v>499</v>
@@ -5709,18 +5711,18 @@
         <v>1282</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>566</v>
+        <v>2133</v>
       </c>
       <c r="B40" s="1">
-        <v>1173</v>
+        <v>2127</v>
       </c>
       <c r="C40" s="1">
-        <v>879</v>
+        <v>3367</v>
       </c>
       <c r="D40" s="1">
         <v>2096</v>
@@ -5732,21 +5734,21 @@
         <v>1531</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>2960</v>
+        <v>2883</v>
       </c>
       <c r="B41" s="1">
-        <v>3281</v>
+        <v>2814</v>
       </c>
       <c r="C41" s="1">
-        <v>3040</v>
+        <v>188</v>
       </c>
       <c r="D41" s="1">
-        <v>2927</v>
+        <v>2883</v>
       </c>
       <c r="E41" s="1">
         <v>3086</v>
@@ -5755,7 +5757,7 @@
         <v>748</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -13445,6 +13447,7 @@
     <mergeCell ref="M6:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
FIX THE NO WORDS LEFT ERROR
</commit_message>
<xml_diff>
--- a/Semantle_AI/New_service/Reports_output/Priority_calculation/error_calc_compare.xlsx
+++ b/Semantle_AI/New_service/Reports_output/Priority_calculation/error_calc_compare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bardamri/PycharmProjects/SE_Project_Semantle/Semantle_AI/New_service/Reports_output/Priority_calculation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA7709B-3F49-B748-9AA0-2F79A871F18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BCD756-FE85-0F41-88EB-46C677EBB13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{2BD9F7E4-3864-E14D-AD8C-55EBE9E46C48}"/>
+    <workbookView xWindow="30240" yWindow="-20340" windowWidth="21600" windowHeight="38400" xr2:uid="{2BD9F7E4-3864-E14D-AD8C-55EBE9E46C48}"/>
   </bookViews>
   <sheets>
     <sheet name="GLOVE_FASTTEXT" sheetId="2" r:id="rId1"/>
@@ -4601,7 +4601,7 @@
   <dimension ref="A1:N1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>